<commit_message>
Added binder logic to recursively bind properties which are classes and lists
</commit_message>
<xml_diff>
--- a/Source/ExcelParser.Tests/ExcelParser.xlsx
+++ b/Source/ExcelParser.Tests/ExcelParser.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Order" sheetId="2" r:id="rId2"/>
+    <sheet name="Address" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Id</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -405,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,8 +438,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -446,8 +461,14 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -464,7 +485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -481,7 +502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -498,7 +519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -522,24 +543,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>